<commit_message>
Pusheo dia 2 maxwell
</commit_message>
<xml_diff>
--- a/Bloque Cuantica-Estadistica/P7 Maxwell/Data.xlsx
+++ b/Bloque Cuantica-Estadistica/P7 Maxwell/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feyra\Desktop\UNI\T-cnicas-experimentales-II\Bloque Cuantica-Estadistica\P7 Maxwell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DD27C7-89F2-4F0C-98FB-0F391AEEC807}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEB6ED7-3BF4-4BFA-9F8A-C5AA730EB46D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1460,7 +1460,7 @@
   <dimension ref="B2:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>